<commit_message>
## Conclusions 4 - smaller learning rate - 0.0001 - Doesn't make much of a difference ### Conclusions going forward: - Need to try with a lot of different params
## Conclusions 5 - baseline for relu
- Batch sizes	Hidden Widths	Nums layers	Functions	Learning rates	Improvement deltas	Improvement patience	Improvement restore weights
    [100]	    [100]	        [4]	        ['relu']	[0.0001]	    [0.001]	            [5]                     [True]
- Local run
- Currently concentrating on train loss: ~.81 (.80-.82)
- Time: ~ 5.4 on average
### Conclusions going forward:
- Use as a baseline
</commit_message>
<xml_diff>
--- a/output/results_2019_08_25_21_39_01_2_loops.xlsx
+++ b/output/results_2019_08_25_21_39_01_2_loops.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Full" sheetId="1" r:id="rId1"/>
@@ -217,10 +217,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -526,72 +532,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:22" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -912,7 +920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>